<commit_message>
cambio con todas las variables sin depuracion
</commit_message>
<xml_diff>
--- a/data/output/datasets/pib_dataset.xlsx
+++ b/data/output/datasets/pib_dataset.xlsx
@@ -1,72 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>exportaciones</t>
-  </si>
-  <si>
-    <t>inversiones</t>
-  </si>
-  <si>
-    <t>gasto_publico</t>
-  </si>
-  <si>
-    <t>consumo_privado</t>
-  </si>
-  <si>
-    <t>importaciones</t>
-  </si>
-  <si>
-    <t>variacion</t>
-  </si>
-  <si>
-    <t>pib</t>
-  </si>
-  <si>
-    <t>fa</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -81,38 +49,96 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -400,1626 +426,1648 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>fa</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>exportaciones</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>inversiones</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>gasto_publico</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>consumo_privado</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>importaciones</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variacion</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>pib</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>39994</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>17180.5</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>12386.8</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>66165.10000000001</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>7645.8</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>22876</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>-5504.4</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>74997.8</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2">
+    <row r="3">
+      <c r="A3" s="2" t="n">
         <v>40086</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>16196.5</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>11359.1</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>65711.89999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>8728.9</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>25296.9</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>-31.9</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>76667.60000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2">
+    <row r="4">
+      <c r="A4" s="2" t="n">
         <v>40178</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>18393.6</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>12432.4</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>67381.60000000001</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>9664.6</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>27584.6</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>-220.7</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>80066.89999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" s="2" t="n">
         <v>40268</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>20262</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>12062.5</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>69048.8</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>7904.4</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>26222.3</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>708.7</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>83764.10000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="2">
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>40359</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="n">
         <v>20276.9</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="n">
         <v>12647</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>70970</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>8587.799999999999</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>28017</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>-3518.4</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="n">
         <v>80946.3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="2">
+    <row r="7">
+      <c r="A7" s="2" t="n">
         <v>40451</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>18265.9</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>12992.1</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>71505.5</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>9372.299999999999</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>29916.7</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="n">
         <v>-51</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="n">
         <v>82168.10000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2">
+    <row r="8">
+      <c r="A8" s="2" t="n">
         <v>40543</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="n">
         <v>20515.3</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>13799.9</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="n">
         <v>74355.2</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>10905.7</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>31771.3</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="n">
         <v>-249.1</v>
       </c>
-      <c r="H8">
+      <c r="H8" t="n">
         <v>87555.7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="2">
+    <row r="9">
+      <c r="A9" s="2" t="n">
         <v>40633</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>23866.7</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>13626.1</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="n">
         <v>76958.7</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>8665.1</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>32232.3</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>576.4</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="n">
         <v>91460.7</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="2">
+    <row r="10">
+      <c r="A10" s="2" t="n">
         <v>40724</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="n">
         <v>22583.7</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="n">
         <v>13823.5</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>76498.5</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>9508.200000000001</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="n">
         <v>33967.6</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="n">
         <v>1176.8</v>
       </c>
-      <c r="H10">
+      <c r="H10" t="n">
         <v>89623.10000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="2">
+    <row r="11">
+      <c r="A11" s="2" t="n">
         <v>40816</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="n">
         <v>22352.8</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="n">
         <v>14684.1</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>80654.7</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>10040.5</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="n">
         <v>35720</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="n">
         <v>48.2</v>
       </c>
-      <c r="H11">
+      <c r="H11" t="n">
         <v>92060.3</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="2">
+    <row r="12">
+      <c r="A12" s="2" t="n">
         <v>40908</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="n">
         <v>22162</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="n">
         <v>15441</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>81055.10000000001</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>11787.5</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="n">
         <v>34100.5</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="n">
         <v>-139.1</v>
       </c>
-      <c r="H12">
+      <c r="H12" t="n">
         <v>96206</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="2">
+    <row r="13">
+      <c r="A13" s="2" t="n">
         <v>40999</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="n">
         <v>24171.8</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="n">
         <v>14820.7</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>84395.5</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>9450</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="n">
         <v>35199.1</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="n">
         <v>507.9</v>
       </c>
-      <c r="H13">
+      <c r="H13" t="n">
         <v>98146.8</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="2">
+    <row r="14">
+      <c r="A14" s="2" t="n">
         <v>41090</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>22011.5</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="n">
         <v>15216.6</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="n">
         <v>81625.5</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>9657.9</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="n">
         <v>34055.8</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="n">
         <v>545.5</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="n">
         <v>95001.2</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="2">
+    <row r="15">
+      <c r="A15" s="2" t="n">
         <v>41182</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>21455.4</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="n">
         <v>15110.2</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="n">
         <v>83050.8</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>10915.8</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="n">
         <v>34474.9</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="n">
         <v>-115.1</v>
       </c>
-      <c r="H15">
+      <c r="H15" t="n">
         <v>95942.2</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="2">
+    <row r="16">
+      <c r="A16" s="2" t="n">
         <v>41274</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>21933.5</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="n">
         <v>16414.4</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>86717.39999999999</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>13415.9</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="n">
         <v>36369.7</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="n">
         <v>-275.7</v>
       </c>
-      <c r="H16">
+      <c r="H16" t="n">
         <v>101835.8</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="2">
+    <row r="17">
+      <c r="A17" s="2" t="n">
         <v>41364</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="n">
         <v>23778.57</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="n">
         <v>14521.32</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="n">
         <v>85731.61</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>9430.139999999999</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="n">
         <v>34315.33</v>
       </c>
-      <c r="G17">
+      <c r="G17" t="n">
         <v>4688.3</v>
       </c>
-      <c r="H17">
+      <c r="H17" t="n">
         <v>103834.61</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="2">
+    <row r="18">
+      <c r="A18" s="2" t="n">
         <v>41455</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="n">
         <v>23284.22</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="n">
         <v>15653.6</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="n">
         <v>88630.94</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>11800.43</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="n">
         <v>36399.45</v>
       </c>
-      <c r="G18">
+      <c r="G18" t="n">
         <v>-793.12</v>
       </c>
-      <c r="H18">
+      <c r="H18" t="n">
         <v>102176.63</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="2">
+    <row r="19">
+      <c r="A19" s="2" t="n">
         <v>41547</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="n">
         <v>21766.35</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="n">
         <v>16060.58</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="n">
         <v>89423.33</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>12004.06</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="n">
         <v>36633.45</v>
       </c>
-      <c r="G19">
+      <c r="G19" t="n">
         <v>-403.61</v>
       </c>
-      <c r="H19">
+      <c r="H19" t="n">
         <v>102217.26</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="2">
+    <row r="20">
+      <c r="A20" s="2" t="n">
         <v>41639</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="n">
         <v>22767.49</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="n">
         <v>16599.08</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="n">
         <v>92464.67</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="n">
         <v>13766.49</v>
       </c>
-      <c r="F20">
+      <c r="F20" t="n">
         <v>37082.89</v>
       </c>
-      <c r="G20">
+      <c r="G20" t="n">
         <v>-360.12</v>
       </c>
-      <c r="H20">
+      <c r="H20" t="n">
         <v>108154.72</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="2">
+    <row r="21">
+      <c r="A21" s="2" t="n">
         <v>41729</v>
       </c>
-      <c r="B21">
+      <c r="B21" t="n">
         <v>24335.8</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="n">
         <v>15781.53</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="n">
         <v>91248.72</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="n">
         <v>10326.9</v>
       </c>
-      <c r="F21">
+      <c r="F21" t="n">
         <v>35612.86</v>
       </c>
-      <c r="G21">
+      <c r="G21" t="n">
         <v>3443.9</v>
       </c>
-      <c r="H21">
+      <c r="H21" t="n">
         <v>109523.98</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="2">
+    <row r="22">
+      <c r="A22" s="2" t="n">
         <v>41820</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="n">
         <v>24870.08</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="n">
         <v>16955.55</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="n">
         <v>94483.36</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="n">
         <v>12334.79</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="n">
         <v>37806.95</v>
       </c>
-      <c r="G22">
+      <c r="G22" t="n">
         <v>-1432.94</v>
       </c>
-      <c r="H22">
+      <c r="H22" t="n">
         <v>109403.88</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="2">
+    <row r="23">
+      <c r="A23" s="2" t="n">
         <v>41912</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="n">
         <v>24269.49</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="n">
         <v>17134.95</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="n">
         <v>96950.88</v>
       </c>
-      <c r="E23">
+      <c r="E23" t="n">
         <v>12904.12</v>
       </c>
-      <c r="F23">
+      <c r="F23" t="n">
         <v>38199.08</v>
       </c>
-      <c r="G23">
+      <c r="G23" t="n">
         <v>-1725.9</v>
       </c>
-      <c r="H23">
+      <c r="H23" t="n">
         <v>111334.46</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="2">
+    <row r="24">
+      <c r="A24" s="2" t="n">
         <v>42004</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="n">
         <v>23792.89</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="n">
         <v>17995.33</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="n">
         <v>98743.28999999999</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="n">
         <v>14782.49</v>
       </c>
-      <c r="F24">
+      <c r="F24" t="n">
         <v>37514.85</v>
       </c>
-      <c r="G24">
+      <c r="G24" t="n">
         <v>-735.14</v>
       </c>
-      <c r="H24">
+      <c r="H24" t="n">
         <v>117064</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="2">
+    <row r="25">
+      <c r="A25" s="2" t="n">
         <v>42094</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="n">
         <v>24243.48</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="n">
         <v>16063.27</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>96635.61</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>11855.61</v>
       </c>
-      <c r="F25">
+      <c r="F25" t="n">
         <v>33930.11</v>
       </c>
-      <c r="G25">
+      <c r="G25" t="n">
         <v>3029.04</v>
       </c>
-      <c r="H25">
+      <c r="H25" t="n">
         <v>117896.91</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="2">
+    <row r="26">
+      <c r="A26" s="2" t="n">
         <v>42185</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="n">
         <v>24496.68</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="n">
         <v>16287.52</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>98920.10000000001</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>12492.36</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="n">
         <v>35436.5</v>
       </c>
-      <c r="G26">
+      <c r="G26" t="n">
         <v>-576.37</v>
       </c>
-      <c r="H26">
+      <c r="H26" t="n">
         <v>116183.79</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="2">
+    <row r="27">
+      <c r="A27" s="2" t="n">
         <v>42277</v>
       </c>
-      <c r="B27">
+      <c r="B27" t="n">
         <v>23367</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="n">
         <v>17793.54</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="n">
         <v>101467.1</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>13431.81</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="n">
         <v>37265.87</v>
       </c>
-      <c r="G27">
+      <c r="G27" t="n">
         <v>-76.89</v>
       </c>
-      <c r="H27">
+      <c r="H27" t="n">
         <v>118716.69</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="2">
+    <row r="28">
+      <c r="A28" s="2" t="n">
         <v>42369</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="n">
         <v>22287.72</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="n">
         <v>18957.91</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="n">
         <v>104347.14</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="n">
         <v>15002.14</v>
       </c>
-      <c r="F28">
+      <c r="F28" t="n">
         <v>36476.86</v>
       </c>
-      <c r="G28">
+      <c r="G28" t="n">
         <v>-892.61</v>
       </c>
-      <c r="H28">
+      <c r="H28" t="n">
         <v>123225.44</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="2">
+    <row r="29">
+      <c r="A29" s="2" t="n">
         <v>42460</v>
       </c>
-      <c r="B29">
+      <c r="B29" t="n">
         <v>23867.37</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="n">
         <v>16061.27</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="n">
         <v>102827.45</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="n">
         <v>11252.32</v>
       </c>
-      <c r="F29">
+      <c r="F29" t="n">
         <v>32290.62</v>
       </c>
-      <c r="G29">
+      <c r="G29" t="n">
         <v>2120.67</v>
       </c>
-      <c r="H29">
+      <c r="H29" t="n">
         <v>123838.47</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="2">
+    <row r="30">
+      <c r="A30" s="2" t="n">
         <v>42551</v>
       </c>
-      <c r="B30">
+      <c r="B30" t="n">
         <v>24118.64</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="n">
         <v>17445.98</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="n">
         <v>105141.61</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="n">
         <v>11552.85</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="n">
         <v>35363.92</v>
       </c>
-      <c r="G30">
+      <c r="G30" t="n">
         <v>-95.84999999999999</v>
       </c>
-      <c r="H30">
+      <c r="H30" t="n">
         <v>122799.32</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="2">
+    <row r="31">
+      <c r="A31" s="2" t="n">
         <v>42643</v>
       </c>
-      <c r="B31">
+      <c r="B31" t="n">
         <v>22703.15</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="n">
         <v>17127.94</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>106775.98</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>13968.34</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="n">
         <v>34730.6</v>
       </c>
-      <c r="G31">
+      <c r="G31" t="n">
         <v>-1326.69</v>
       </c>
-      <c r="H31">
+      <c r="H31" t="n">
         <v>124518.11</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="2">
+    <row r="32">
+      <c r="A32" s="2" t="n">
         <v>42735</v>
       </c>
-      <c r="B32">
+      <c r="B32" t="n">
         <v>23451.67</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="n">
         <v>19001.06</v>
       </c>
-      <c r="D32">
+      <c r="D32" t="n">
         <v>109768.87</v>
       </c>
-      <c r="E32">
+      <c r="E32" t="n">
         <v>15637.24</v>
       </c>
-      <c r="F32">
+      <c r="F32" t="n">
         <v>36265.97</v>
       </c>
-      <c r="G32">
+      <c r="G32" t="n">
         <v>-747.0599999999999</v>
       </c>
-      <c r="H32">
+      <c r="H32" t="n">
         <v>130845.8</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="2">
+    <row r="33">
+      <c r="A33" s="2" t="n">
         <v>42825</v>
       </c>
-      <c r="B33">
+      <c r="B33" t="n">
         <v>25904.65</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="n">
         <v>16797.89</v>
       </c>
-      <c r="D33">
+      <c r="D33" t="n">
         <v>108265.29</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="n">
         <v>11742.32</v>
       </c>
-      <c r="F33">
+      <c r="F33" t="n">
         <v>34647.15</v>
       </c>
-      <c r="G33">
+      <c r="G33" t="n">
         <v>3619.7</v>
       </c>
-      <c r="H33">
+      <c r="H33" t="n">
         <v>131682.69</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="2">
+    <row r="34">
+      <c r="A34" s="2" t="n">
         <v>42916</v>
       </c>
-      <c r="B34">
+      <c r="B34" t="n">
         <v>24993.89</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="n">
         <v>17179.23</v>
       </c>
-      <c r="D34">
+      <c r="D34" t="n">
         <v>109436.69</v>
       </c>
-      <c r="E34">
+      <c r="E34" t="n">
         <v>11995.86</v>
       </c>
-      <c r="F34">
+      <c r="F34" t="n">
         <v>34858.4</v>
       </c>
-      <c r="G34">
+      <c r="G34" t="n">
         <v>-1096.96</v>
       </c>
-      <c r="H34">
+      <c r="H34" t="n">
         <v>127650.31</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="2">
+    <row r="35">
+      <c r="A35" s="2" t="n">
         <v>43008</v>
       </c>
-      <c r="B35">
+      <c r="B35" t="n">
         <v>23188.11</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="n">
         <v>18703.37</v>
       </c>
-      <c r="D35">
+      <c r="D35" t="n">
         <v>112095.83</v>
       </c>
-      <c r="E35">
+      <c r="E35" t="n">
         <v>14345.69</v>
       </c>
-      <c r="F35">
+      <c r="F35" t="n">
         <v>35960.84</v>
       </c>
-      <c r="G35">
+      <c r="G35" t="n">
         <v>-2080.41</v>
       </c>
-      <c r="H35">
+      <c r="H35" t="n">
         <v>130291.75</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="2">
+    <row r="36">
+      <c r="A36" s="2" t="n">
         <v>43100</v>
       </c>
-      <c r="B36">
+      <c r="B36" t="n">
         <v>23291.14</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="n">
         <v>18974.17</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="n">
         <v>117261.74</v>
       </c>
-      <c r="E36">
+      <c r="E36" t="n">
         <v>17582.83</v>
       </c>
-      <c r="F36">
+      <c r="F36" t="n">
         <v>39714.73</v>
       </c>
-      <c r="G36">
+      <c r="G36" t="n">
         <v>-512.48</v>
       </c>
-      <c r="H36">
+      <c r="H36" t="n">
         <v>136882.66</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="2">
+    <row r="37">
+      <c r="A37" s="2" t="n">
         <v>43190</v>
       </c>
-      <c r="B37">
+      <c r="B37" t="n">
         <v>25389.07</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="n">
         <v>17034</v>
       </c>
-      <c r="D37">
+      <c r="D37" t="n">
         <v>113161.65</v>
       </c>
-      <c r="E37">
+      <c r="E37" t="n">
         <v>12758.97</v>
       </c>
-      <c r="F37">
+      <c r="F37" t="n">
         <v>35608.78</v>
       </c>
-      <c r="G37">
+      <c r="G37" t="n">
         <v>4213.34</v>
       </c>
-      <c r="H37">
+      <c r="H37" t="n">
         <v>136948.25</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="2">
+    <row r="38">
+      <c r="A38" s="2" t="n">
         <v>43281</v>
       </c>
-      <c r="B38">
+      <c r="B38" t="n">
         <v>25476.24</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="n">
         <v>18725</v>
       </c>
-      <c r="D38">
+      <c r="D38" t="n">
         <v>115969.39</v>
       </c>
-      <c r="E38">
+      <c r="E38" t="n">
         <v>13812.74</v>
       </c>
-      <c r="F38">
+      <c r="F38" t="n">
         <v>40255.53</v>
       </c>
-      <c r="G38">
+      <c r="G38" t="n">
         <v>860.85</v>
       </c>
-      <c r="H38">
+      <c r="H38" t="n">
         <v>134588.69</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="2">
+    <row r="39">
+      <c r="A39" s="2" t="n">
         <v>43373</v>
       </c>
-      <c r="B39">
+      <c r="B39" t="n">
         <v>24666.81</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="n">
         <v>19486.35</v>
       </c>
-      <c r="D39">
+      <c r="D39" t="n">
         <v>119179.46</v>
       </c>
-      <c r="E39">
+      <c r="E39" t="n">
         <v>16109.34</v>
       </c>
-      <c r="F39">
+      <c r="F39" t="n">
         <v>40584.92</v>
       </c>
-      <c r="G39">
+      <c r="G39" t="n">
         <v>-2407.14</v>
       </c>
-      <c r="H39">
+      <c r="H39" t="n">
         <v>136449.9</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="2">
+    <row r="40">
+      <c r="A40" s="2" t="n">
         <v>43465</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="n">
         <v>24647.75</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="n">
         <v>20269.45</v>
       </c>
-      <c r="D40">
+      <c r="D40" t="n">
         <v>124555.71</v>
       </c>
-      <c r="E40">
+      <c r="E40" t="n">
         <v>18632.5</v>
       </c>
-      <c r="F40">
+      <c r="F40" t="n">
         <v>42578.31</v>
       </c>
-      <c r="G40">
+      <c r="G40" t="n">
         <v>-2145.85</v>
       </c>
-      <c r="H40">
+      <c r="H40" t="n">
         <v>143381.24</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="2">
+    <row r="41">
+      <c r="A41" s="2" t="n">
         <v>43555</v>
       </c>
-      <c r="B41">
+      <c r="B41" t="n">
         <v>26350.63</v>
       </c>
-      <c r="C41">
+      <c r="C41" t="n">
         <v>18858.3</v>
       </c>
-      <c r="D41">
+      <c r="D41" t="n">
         <v>121527.27</v>
       </c>
-      <c r="E41">
+      <c r="E41" t="n">
         <v>13665.33</v>
       </c>
-      <c r="F41">
+      <c r="F41" t="n">
         <v>39631.34</v>
       </c>
-      <c r="G41">
+      <c r="G41" t="n">
         <v>4156.63</v>
       </c>
-      <c r="H41">
+      <c r="H41" t="n">
         <v>144926.83</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="2">
+    <row r="42">
+      <c r="A42" s="2" t="n">
         <v>43646</v>
       </c>
-      <c r="B42">
+      <c r="B42" t="n">
         <v>26529.72</v>
       </c>
-      <c r="C42">
+      <c r="C42" t="n">
         <v>21780.48</v>
       </c>
-      <c r="D42">
+      <c r="D42" t="n">
         <v>124206.7</v>
       </c>
-      <c r="E42">
+      <c r="E42" t="n">
         <v>14609.2</v>
       </c>
-      <c r="F42">
+      <c r="F42" t="n">
         <v>40851.34</v>
       </c>
-      <c r="G42">
+      <c r="G42" t="n">
         <v>-925.61</v>
       </c>
-      <c r="H42">
+      <c r="H42" t="n">
         <v>145349.16</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="2">
+    <row r="43">
+      <c r="A43" s="2" t="n">
         <v>43738</v>
       </c>
-      <c r="B43">
+      <c r="B43" t="n">
         <v>25727.8</v>
       </c>
-      <c r="C43">
+      <c r="C43" t="n">
         <v>21907.27</v>
       </c>
-      <c r="D43">
+      <c r="D43" t="n">
         <v>126417.03</v>
       </c>
-      <c r="E43">
+      <c r="E43" t="n">
         <v>17509.59</v>
       </c>
-      <c r="F43">
+      <c r="F43" t="n">
         <v>41482.82</v>
       </c>
-      <c r="G43">
+      <c r="G43" t="n">
         <v>-2448.4</v>
       </c>
-      <c r="H43">
+      <c r="H43" t="n">
         <v>147630.47</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="2">
+    <row r="44">
+      <c r="A44" s="2" t="n">
         <v>43830</v>
       </c>
-      <c r="B44">
+      <c r="B44" t="n">
         <v>26002.06</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="n">
         <v>22862.93</v>
       </c>
-      <c r="D44">
+      <c r="D44" t="n">
         <v>131869.59</v>
       </c>
-      <c r="E44">
+      <c r="E44" t="n">
         <v>20188.38</v>
       </c>
-      <c r="F44">
+      <c r="F44" t="n">
         <v>43781.01</v>
       </c>
-      <c r="G44">
+      <c r="G44" t="n">
         <v>-1076.38</v>
       </c>
-      <c r="H44">
+      <c r="H44" t="n">
         <v>156065.57</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="2">
+    <row r="45">
+      <c r="A45" s="2" t="n">
         <v>43921</v>
       </c>
-      <c r="B45">
+      <c r="B45" t="n">
         <v>27538.38</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="n">
         <v>19336.23</v>
       </c>
-      <c r="D45">
+      <c r="D45" t="n">
         <v>124497.43</v>
       </c>
-      <c r="E45">
+      <c r="E45" t="n">
         <v>14332.93</v>
       </c>
-      <c r="F45">
+      <c r="F45" t="n">
         <v>39435.21</v>
       </c>
-      <c r="G45">
+      <c r="G45" t="n">
         <v>5008.19</v>
       </c>
-      <c r="H45">
+      <c r="H45" t="n">
         <v>151277.95</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="2">
+    <row r="46">
+      <c r="A46" s="2" t="n">
         <v>44012</v>
       </c>
-      <c r="B46">
+      <c r="B46" t="n">
         <v>21895.37</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="n">
         <v>18519.86</v>
       </c>
-      <c r="D46">
+      <c r="D46" t="n">
         <v>113987.8</v>
       </c>
-      <c r="E46">
+      <c r="E46" t="n">
         <v>14897.08</v>
       </c>
-      <c r="F46">
+      <c r="F46" t="n">
         <v>31400.47</v>
       </c>
-      <c r="G46">
+      <c r="G46" t="n">
         <v>-1387.1</v>
       </c>
-      <c r="H46">
+      <c r="H46" t="n">
         <v>136512.54</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="2">
+    <row r="47">
+      <c r="A47" s="2" t="n">
         <v>44104</v>
       </c>
-      <c r="B47">
+      <c r="B47" t="n">
         <v>23306.82</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="n">
         <v>21291.87</v>
       </c>
-      <c r="D47">
+      <c r="D47" t="n">
         <v>126716.85</v>
       </c>
-      <c r="E47">
+      <c r="E47" t="n">
         <v>17888.81</v>
       </c>
-      <c r="F47">
+      <c r="F47" t="n">
         <v>35680.23</v>
       </c>
-      <c r="G47">
+      <c r="G47" t="n">
         <v>-3383.02</v>
       </c>
-      <c r="H47">
+      <c r="H47" t="n">
         <v>150141.09</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="2">
+    <row r="48">
+      <c r="A48" s="2" t="n">
         <v>44196</v>
       </c>
-      <c r="B48">
+      <c r="B48" t="n">
         <v>25341.13</v>
       </c>
-      <c r="C48">
+      <c r="C48" t="n">
         <v>23083.59</v>
       </c>
-      <c r="D48">
+      <c r="D48" t="n">
         <v>135785.48</v>
       </c>
-      <c r="E48">
+      <c r="E48" t="n">
         <v>21727.07</v>
       </c>
-      <c r="F48">
+      <c r="F48" t="n">
         <v>42297.36</v>
       </c>
-      <c r="G48">
+      <c r="G48" t="n">
         <v>-1448.98</v>
       </c>
-      <c r="H48">
+      <c r="H48" t="n">
         <v>162190.93</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="2">
+    <row r="49">
+      <c r="A49" s="2" t="n">
         <v>44286</v>
       </c>
-      <c r="B49">
+      <c r="B49" t="n">
         <v>28225.76</v>
       </c>
-      <c r="C49">
+      <c r="C49" t="n">
         <v>24280.23</v>
       </c>
-      <c r="D49">
+      <c r="D49" t="n">
         <v>137035.27</v>
       </c>
-      <c r="E49">
+      <c r="E49" t="n">
         <v>15335.99</v>
       </c>
-      <c r="F49">
+      <c r="F49" t="n">
         <v>45182.97</v>
       </c>
-      <c r="G49">
+      <c r="G49" t="n">
         <v>3179.45</v>
       </c>
-      <c r="H49">
+      <c r="H49" t="n">
         <v>162873.72</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="2">
+    <row r="50">
+      <c r="A50" s="2" t="n">
         <v>44377</v>
       </c>
-      <c r="B50">
+      <c r="B50" t="n">
         <v>29053.21</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="n">
         <v>26063.64</v>
       </c>
-      <c r="D50">
+      <c r="D50" t="n">
         <v>138196.2</v>
       </c>
-      <c r="E50">
+      <c r="E50" t="n">
         <v>16965.33</v>
       </c>
-      <c r="F50">
+      <c r="F50" t="n">
         <v>51033.38</v>
       </c>
-      <c r="G50">
+      <c r="G50" t="n">
         <v>2846.32</v>
       </c>
-      <c r="H50">
+      <c r="H50" t="n">
         <v>162091.32</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="2">
+    <row r="51">
+      <c r="A51" s="2" t="n">
         <v>44469</v>
       </c>
-      <c r="B51">
+      <c r="B51" t="n">
         <v>30006.58</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="n">
         <v>28472.39</v>
       </c>
-      <c r="D51">
+      <c r="D51" t="n">
         <v>144978.03</v>
       </c>
-      <c r="E51">
+      <c r="E51" t="n">
         <v>19303.82</v>
       </c>
-      <c r="F51">
+      <c r="F51" t="n">
         <v>54700.43</v>
       </c>
-      <c r="G51">
+      <c r="G51" t="n">
         <v>-825.85</v>
       </c>
-      <c r="H51">
+      <c r="H51" t="n">
         <v>167234.54</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="2">
+    <row r="52">
+      <c r="A52" s="2" t="n">
         <v>44561</v>
       </c>
-      <c r="B52">
+      <c r="B52" t="n">
         <v>30600.54</v>
       </c>
-      <c r="C52">
+      <c r="C52" t="n">
         <v>29050.01</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="n">
         <v>154904.38</v>
       </c>
-      <c r="E52">
+      <c r="E52" t="n">
         <v>23503.51</v>
       </c>
-      <c r="F52">
+      <c r="F52" t="n">
         <v>60596.87</v>
       </c>
-      <c r="G52">
+      <c r="G52" t="n">
         <v>-800.28</v>
       </c>
-      <c r="H52">
+      <c r="H52" t="n">
         <v>176661.29</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="2">
+    <row r="53">
+      <c r="A53" s="2" t="n">
         <v>44651</v>
       </c>
-      <c r="B53">
+      <c r="B53" t="n">
         <v>34901.81</v>
       </c>
-      <c r="C53">
+      <c r="C53" t="n">
         <v>29800.35</v>
       </c>
-      <c r="D53">
+      <c r="D53" t="n">
         <v>154730.28</v>
       </c>
-      <c r="E53">
+      <c r="E53" t="n">
         <v>17180.01</v>
       </c>
-      <c r="F53">
+      <c r="F53" t="n">
         <v>62183.18</v>
       </c>
-      <c r="G53">
+      <c r="G53" t="n">
         <v>5043.77</v>
       </c>
-      <c r="H53">
+      <c r="H53" t="n">
         <v>179473.04</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="2">
+    <row r="54">
+      <c r="A54" s="2" t="n">
         <v>44742</v>
       </c>
-      <c r="B54">
+      <c r="B54" t="n">
         <v>36763.29</v>
       </c>
-      <c r="C54">
+      <c r="C54" t="n">
         <v>29923.77</v>
       </c>
-      <c r="D54">
+      <c r="D54" t="n">
         <v>159866.86</v>
       </c>
-      <c r="E54">
+      <c r="E54" t="n">
         <v>18950.02</v>
       </c>
-      <c r="F54">
+      <c r="F54" t="n">
         <v>67025.05</v>
       </c>
-      <c r="G54">
+      <c r="G54" t="n">
         <v>1058.88</v>
       </c>
-      <c r="H54">
+      <c r="H54" t="n">
         <v>179537.77</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="2">
+    <row r="55">
+      <c r="A55" s="2" t="n">
         <v>44834</v>
       </c>
-      <c r="B55">
+      <c r="B55" t="n">
         <v>34988.86</v>
       </c>
-      <c r="C55">
+      <c r="C55" t="n">
         <v>31955.14</v>
       </c>
-      <c r="D55">
+      <c r="D55" t="n">
         <v>166286.69</v>
       </c>
-      <c r="E55">
+      <c r="E55" t="n">
         <v>21881.11</v>
       </c>
-      <c r="F55">
+      <c r="F55" t="n">
         <v>68476.07000000001</v>
       </c>
-      <c r="G55">
+      <c r="G55" t="n">
         <v>-1020.46</v>
       </c>
-      <c r="H55">
+      <c r="H55" t="n">
         <v>185615.28</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="2">
+    <row r="56">
+      <c r="A56" s="2" t="n">
         <v>44926</v>
       </c>
-      <c r="B56">
+      <c r="B56" t="n">
         <v>33742.28</v>
       </c>
-      <c r="C56">
+      <c r="C56" t="n">
         <v>32093.43</v>
       </c>
-      <c r="D56">
+      <c r="D56" t="n">
         <v>174720.37</v>
       </c>
-      <c r="E56">
+      <c r="E56" t="n">
         <v>27019.03</v>
       </c>
-      <c r="F56">
+      <c r="F56" t="n">
         <v>65249.7</v>
       </c>
-      <c r="G56">
+      <c r="G56" t="n">
         <v>-5982.86</v>
       </c>
-      <c r="H56">
+      <c r="H56" t="n">
         <v>196342.55</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="2">
+    <row r="57">
+      <c r="A57" s="2" t="n">
         <v>45016</v>
       </c>
-      <c r="B57">
+      <c r="B57" t="n">
         <v>36177.39</v>
       </c>
-      <c r="C57">
+      <c r="C57" t="n">
         <v>31896.19</v>
       </c>
-      <c r="D57">
+      <c r="D57" t="n">
         <v>172616.53</v>
       </c>
-      <c r="E57">
+      <c r="E57" t="n">
         <v>20622.29</v>
       </c>
-      <c r="F57">
+      <c r="F57" t="n">
         <v>61820.93</v>
       </c>
-      <c r="G57">
+      <c r="G57" t="n">
         <v>1320.93</v>
       </c>
-      <c r="H57">
+      <c r="H57" t="n">
         <v>200812.4</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="2">
+    <row r="58">
+      <c r="A58" s="2" t="n">
         <v>45107</v>
       </c>
-      <c r="B58">
+      <c r="B58" t="n">
         <v>34678.17</v>
       </c>
-      <c r="C58">
+      <c r="C58" t="n">
         <v>31663.98</v>
       </c>
-      <c r="D58">
+      <c r="D58" t="n">
         <v>175761.43</v>
       </c>
-      <c r="E58">
+      <c r="E58" t="n">
         <v>23129.23</v>
       </c>
-      <c r="F58">
+      <c r="F58" t="n">
         <v>64363.65</v>
       </c>
-      <c r="G58">
+      <c r="G58" t="n">
         <v>-21.74</v>
       </c>
-      <c r="H58">
+      <c r="H58" t="n">
         <v>200847.42</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="2">
+    <row r="59">
+      <c r="A59" s="2" t="n">
         <v>45199</v>
       </c>
-      <c r="B59">
+      <c r="B59" t="n">
         <v>33039.01</v>
       </c>
-      <c r="C59">
+      <c r="C59" t="n">
         <v>34766.21</v>
       </c>
-      <c r="D59">
+      <c r="D59" t="n">
         <v>179216.82</v>
       </c>
-      <c r="E59">
+      <c r="E59" t="n">
         <v>23189.9</v>
       </c>
-      <c r="F59">
+      <c r="F59" t="n">
         <v>66146.42</v>
       </c>
-      <c r="G59">
+      <c r="G59" t="n">
         <v>-367.91</v>
       </c>
-      <c r="H59">
+      <c r="H59" t="n">
         <v>203697.61</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="2">
+    <row r="60">
+      <c r="A60" s="2" t="n">
         <v>45291</v>
       </c>
-      <c r="B60">
+      <c r="B60" t="n">
         <v>31587.4</v>
       </c>
-      <c r="C60">
+      <c r="C60" t="n">
         <v>34067.36</v>
       </c>
-      <c r="D60">
+      <c r="D60" t="n">
         <v>187342.98</v>
       </c>
-      <c r="E60">
+      <c r="E60" t="n">
         <v>24929.79</v>
       </c>
-      <c r="F60">
+      <c r="F60" t="n">
         <v>66394.61</v>
       </c>
-      <c r="G60">
+      <c r="G60" t="n">
         <v>1163.69</v>
       </c>
-      <c r="H60">
+      <c r="H60" t="n">
         <v>212696.62</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="2">
+    <row r="61">
+      <c r="A61" s="2" t="n">
         <v>45382</v>
       </c>
-      <c r="B61">
+      <c r="B61" t="n">
         <v>34838.92</v>
       </c>
-      <c r="C61">
+      <c r="C61" t="n">
         <v>32898.42</v>
       </c>
-      <c r="D61">
+      <c r="D61" t="n">
         <v>186251.67</v>
       </c>
-      <c r="E61">
+      <c r="E61" t="n">
         <v>20670.85</v>
       </c>
-      <c r="F61">
+      <c r="F61" t="n">
         <v>66138.42999999999</v>
       </c>
-      <c r="G61">
+      <c r="G61" t="n">
         <v>6524.68</v>
       </c>
-      <c r="H61">
+      <c r="H61" t="n">
         <v>215046.12</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="2">
+    <row r="62">
+      <c r="A62" s="2" t="n">
         <v>45473</v>
       </c>
-      <c r="B62">
+      <c r="B62" t="n">
         <v>36378.46</v>
       </c>
-      <c r="C62">
+      <c r="C62" t="n">
         <v>33643.2</v>
       </c>
-      <c r="D62">
+      <c r="D62" t="n">
         <v>190042.81</v>
       </c>
-      <c r="E62">
+      <c r="E62" t="n">
         <v>21631.61</v>
       </c>
-      <c r="F62">
+      <c r="F62" t="n">
         <v>69394.14999999999</v>
       </c>
-      <c r="G62">
+      <c r="G62" t="n">
         <v>1707.4</v>
       </c>
-      <c r="H62">
+      <c r="H62" t="n">
         <v>214009.32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>